<commit_message>
parseGPmarkdown helper function now works with compileProcedure function to expand {vid 3} shorthand to [▶\"Lesson Trailer: \"Females Singing to be Heard\"\"](https://www.youtube.com/watch?v=HSBO60ZNeCo&list=PLz-D3xOC0d8-6cZe7bbKs1ItYJHTBaFuP&index=3)
</commit_message>
<xml_diff>
--- a/meta/procedure.xlsx
+++ b/meta/procedure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattwilkins/mrw_synced/R/Nonshiny Github/galacticPubs/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38527746-D428-7848-BE10-CBCCC49AD409}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D363DA-86F4-2F40-BE65-A358966F94A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -244,7 +244,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="121">
   <si>
     <t>Part</t>
   </si>
@@ -625,6 +625,9 @@
   </si>
   <si>
     <t>All the videos {vid7}, {vid6}, {vid    1}, {vid10}, {vid12}</t>
+  </si>
+  <si>
+    <t>I'm mentioning {vid 1} here, and a vid that doesn't exist ({vid33})</t>
   </si>
 </sst>
 </file>
@@ -8201,7 +8204,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -8313,7 +8316,9 @@
       <c r="I2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="19"/>
+      <c r="J2" s="19" t="s">
+        <v>120</v>
+      </c>
       <c r="K2" s="20" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
al final, lo hice
</commit_message>
<xml_diff>
--- a/meta/procedure.xlsx
+++ b/meta/procedure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattwilkins/mrw_synced/R/Nonshiny Github/galacticPubs/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D363DA-86F4-2F40-BE65-A358966F94A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2FD75E-E84F-E14A-BFBF-BF35FA275B9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,6 +100,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
+    <author>Matt Wilkins</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
@@ -163,9 +164,25 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Concise description (used in "Teach it in 15" Presentation)
-*To insert a link to 1 of our vids, use {vid1} for video 1 on the teaching-links.xlsx file
-======</t>
+          <t xml:space="preserve">Concise description (used in "Teach it in 15" Presentation)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">*To insert a link to 1 of our vids, use {vid1} for video 1 on the teaching-links.xlsx file
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>======</t>
         </r>
       </text>
     </comment>
@@ -196,6 +213,19 @@
             <rFont val="Arial"/>
           </rPr>
           <t>======</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{39B9F457-6D4C-C148-A479-595FB846C7A7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use word=def (alt+enter to make new line) for each entry. It'll be formatted into bullets</t>
         </r>
       </text>
     </comment>
@@ -326,14 +356,6 @@
   <si>
     <t>By spending some time introducing students to ciphers, we laying the groundwork for cipher-based puzzle hooks for each part of this lesson. The Polymath Puzzle in Part 1 draws students into decoding the labels on a graph in order to engage them in trying to understand the next level of meaning in the graph, creating a rich data literacy learning experience. In the first step, students learn that ciphers are used to make a secret message. We use a simple cipher called an alphabetic shift, where each letter of each word in a message has been shifted a certain number of places (e.g. +1 would mean A becomes B, B becomes C, and so on).
 This section works on assimilating new vocabulary, as well as encouraging students to have a growth mindset. They need to quickly orient themselves to the "system" of ciphers and how they work. Parts 2 and 3 of the lesson will build on this engagement hook.</t>
-  </si>
-  <si>
-    <t>- **algorithm:** a set of steps, like a mathematical recipe
-- **alphabetic shift:** type of cipher where each letter has been shifted a certain number of places (dictated by the algorithm)
-- **cipher:** a secret message that uses an algorithm to make a message seem like nonsense
-- **decipher:** 1) to convert a secret message into readable text; 2) to succeed in understanding something 
-- **encipher:** convert readable text (plaintext) into a secret message
-- **plaintext:** readable text (not a cipher)</t>
   </si>
   <si>
     <t>Ask students to read slides and predict what the next slide will be (e.g. the next letter in the alphabetic shift). Model a growth mindset, and that it's ok to not completely understand at first.</t>
@@ -629,12 +651,20 @@
   <si>
     <t>I'm mentioning {vid 1} here, and a vid that doesn't exist ({vid33})</t>
   </si>
+  <si>
+    <t>algorithm =   a set of steps, like a mathematical recipe
+alphabetic shift= type of cipher where each letter has been shifted a certain number of places (dictated by the algorithm)
+- **cipher:** a secret message that uses an algorithm to make a message seem like nonsense
+- **decipher:** 1) to convert a secret message into readable text; 2) to succeed in understanding something 
+- **encipher:** convert readable text (plaintext) into a secret message
+- **plaintext:** readable text (not a cipher)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -706,6 +736,12 @@
     <font>
       <sz val="10"/>
       <name val="Roboto Mono"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -915,6 +951,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8204,7 +8244,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -8308,19 +8348,19 @@
         <v>25</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H2" s="20" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>28</v>
       </c>
       <c r="M2" s="21">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("unique(A2:A1000)"),1)</f>
@@ -8351,18 +8391,18 @@
         <v>2</v>
       </c>
       <c r="F3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>29</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>30</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="24"/>
       <c r="J3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="M3" s="25">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2)</f>
@@ -8391,24 +8431,24 @@
         <v>10</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="20">
         <v>3</v>
       </c>
       <c r="F4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>34</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>35</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="20"/>
       <c r="J4" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="20" t="s">
         <v>36</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>37</v>
       </c>
       <c r="M4" s="25">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3)</f>
@@ -8439,15 +8479,15 @@
         <v>4</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" s="19"/>
       <c r="M5" s="25"/>
@@ -8470,26 +8510,26 @@
         <v>15</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="20">
         <v>5</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>42</v>
       </c>
       <c r="I6" s="24"/>
       <c r="J6" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>44</v>
       </c>
       <c r="M6" s="21"/>
       <c r="N6" s="26"/>
@@ -8513,10 +8553,10 @@
         <v>6</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="19"/>
@@ -8542,22 +8582,22 @@
         <v>5</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="20">
         <v>7</v>
       </c>
       <c r="F8" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="H8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="I8" s="24" t="s">
         <v>49</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>50</v>
       </c>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
@@ -8583,13 +8623,13 @@
         <v>8</v>
       </c>
       <c r="F9" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>52</v>
       </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
@@ -8616,13 +8656,13 @@
         <v>9</v>
       </c>
       <c r="F10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="H10" s="20" t="s">
         <v>54</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>55</v>
       </c>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
@@ -8647,19 +8687,19 @@
         <v>10</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="20">
         <v>1</v>
       </c>
       <c r="F11" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="H11" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
@@ -8684,16 +8724,16 @@
         <v>5</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="20">
         <v>2</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
@@ -8719,20 +8759,20 @@
         <v>15</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="20">
         <v>3</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
@@ -8758,10 +8798,10 @@
         <v>4</v>
       </c>
       <c r="F14" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>63</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>64</v>
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
@@ -8789,13 +8829,13 @@
         <v>5</v>
       </c>
       <c r="F15" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>65</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>66</v>
       </c>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
@@ -8820,16 +8860,16 @@
         <v>10</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="20">
         <v>6</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
@@ -8855,16 +8895,16 @@
         <v>5</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" s="20">
         <v>7</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
@@ -8892,18 +8932,18 @@
         <v>8</v>
       </c>
       <c r="F18" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="H18" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M18" s="21"/>
       <c r="N18" s="26"/>
@@ -8925,22 +8965,22 @@
         <v>5</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="20">
         <v>1</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M19" s="21"/>
       <c r="N19" s="26"/>
@@ -8964,10 +9004,10 @@
         <v>2</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
@@ -8993,16 +9033,16 @@
         <v>10</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" s="20">
         <v>3</v>
       </c>
       <c r="F21" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="20" t="s">
         <v>80</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>81</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
@@ -9030,10 +9070,10 @@
         <v>4</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
@@ -9061,10 +9101,10 @@
         <v>5</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
@@ -9090,16 +9130,16 @@
         <v>10</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24" s="20">
         <v>6</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
@@ -9127,10 +9167,10 @@
         <v>7</v>
       </c>
       <c r="F25" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>87</v>
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
@@ -9158,15 +9198,15 @@
         <v>8</v>
       </c>
       <c r="F26" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="20" t="s">
         <v>88</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>89</v>
       </c>
       <c r="H26" s="19"/>
       <c r="I26" s="24"/>
       <c r="J26" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K26" s="19"/>
       <c r="M26" s="21"/>
@@ -9189,24 +9229,24 @@
         <v>5</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" s="20">
         <v>9</v>
       </c>
       <c r="F27" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="H27" s="24" t="s">
         <v>93</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>94</v>
       </c>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
       <c r="K27" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M27" s="21"/>
       <c r="N27" s="26"/>
@@ -9228,24 +9268,24 @@
         <v>5</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E28" s="20">
         <v>10</v>
       </c>
       <c r="F28" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>98</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="K28" s="20" t="s">
         <v>99</v>
-      </c>
-      <c r="K28" s="20" t="s">
-        <v>100</v>
       </c>
       <c r="M28" s="21"/>
       <c r="N28" s="26"/>
@@ -9267,16 +9307,16 @@
         <v>10</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E29" s="20">
         <v>11</v>
       </c>
       <c r="F29" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="20" t="s">
         <v>102</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>103</v>
       </c>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
@@ -9304,15 +9344,15 @@
         <v>12</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K30" s="19"/>
       <c r="M30" s="21"/>
@@ -9337,16 +9377,16 @@
         <v>13</v>
       </c>
       <c r="F31" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>107</v>
       </c>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
       <c r="K31" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M31" s="21"/>
       <c r="N31" s="26"/>

</xml_diff>

<commit_message>
rough draft of classroom Teaching materials done. Also changed name of teaching-material-links to teaching-materials.xlsx
</commit_message>
<xml_diff>
--- a/meta/procedure.xlsx
+++ b/meta/procedure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattwilkins/mrw_synced/R/Nonshiny Github/galacticPubs/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22948E88-3E82-3648-8186-B8D006DE6275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A051F270-CF63-304E-9394-1EF51ADAD33C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="860" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NamesAndNotes" sheetId="1" r:id="rId1"/>
@@ -1269,7 +1269,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1340,74 +1340,6 @@
         <patternFill patternType="solid">
           <bgColor rgb="FF666666"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF4A86E8"/>
-          <bgColor rgb="FF4A86E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCFE2F3"/>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D2E9"/>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4A7D6"/>
-          <bgColor rgb="FFB4A7D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF00FF"/>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9FC5E8"/>
-          <bgColor rgb="FF9FC5E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF00FFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE06666"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
       </fill>
     </dxf>
   </dxfs>
@@ -1631,9 +1563,9 @@
   </sheetPr>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -9720,11 +9652,11 @@
   </sheetPr>
   <dimension ref="A1:AG1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
compileTeachingMat works for both classroom and remote
</commit_message>
<xml_diff>
--- a/meta/procedure.xlsx
+++ b/meta/procedure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattwilkins/mrw_synced/R/Nonshiny Github/galacticPubs/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A051F270-CF63-304E-9394-1EF51ADAD33C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88A2DA3-7684-244D-99FF-44EBCAE05843}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="860" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1565,7 +1565,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:D4"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>

</xml_diff>